<commit_message>
updated outputs, changed axis to 0.01
</commit_message>
<xml_diff>
--- a/outputs/threshold.xlsx
+++ b/outputs/threshold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanxinli/Desktop/project/BlindKameris-new/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A80586F-38A5-044E-820F-D6B424ABF7B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A7F5CC-6472-1347-8183-B0F6F64C3884}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="15880" xr2:uid="{938D64BA-55B7-A240-AE83-1CA07404E743}"/>
+    <workbookView xWindow="3420" yWindow="2120" windowWidth="28040" windowHeight="15880" xr2:uid="{938D64BA-55B7-A240-AE83-1CA07404E743}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>o__Bacteroidales</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>d__Bacteria_include_p__Firmicutes_A</t>
-  </si>
-  <si>
-    <t>not clear</t>
   </si>
 </sst>
 </file>
@@ -421,7 +418,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,8 +459,8 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="D5">
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added hist to outputs
</commit_message>
<xml_diff>
--- a/outputs/threshold.xlsx
+++ b/outputs/threshold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanxinli/Desktop/project/BlindKameris-new/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45EA613-890C-5449-9F0B-08282A4F3C77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EB6C02-3649-2D4D-8109-3C729D11A662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="460" windowWidth="28040" windowHeight="15880" xr2:uid="{938D64BA-55B7-A240-AE83-1CA07404E743}"/>
+    <workbookView xWindow="2560" yWindow="2200" windowWidth="28040" windowHeight="15880" xr2:uid="{938D64BA-55B7-A240-AE83-1CA07404E743}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>o__Bacteroidales</t>
   </si>
@@ -75,10 +75,13 @@
     <t>many instances should not have been rejected, with some rejection 100%</t>
   </si>
   <si>
-    <t>rejection rate for f__Lachnospiraceae is low</t>
-  </si>
-  <si>
     <t>threshold by 0.8 causes low accuracy for g__Ruminocuccues, threshold by 0.7 since 0.7 makes the precision high for most -b datasets</t>
+  </si>
+  <si>
+    <t>seems fine</t>
+  </si>
+  <si>
+    <t>rejection rate for f__Lachnospiraceae is high</t>
   </si>
 </sst>
 </file>
@@ -430,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF1079D-0AAF-A946-91CA-E3C3D76DAEFE}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -449,7 +452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -457,7 +460,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -468,7 +471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -478,8 +481,11 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -487,7 +493,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -495,10 +501,10 @@
         <v>0.8</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -506,10 +512,10 @@
         <v>0.7</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -517,7 +523,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
updated outputs and threshold
</commit_message>
<xml_diff>
--- a/outputs/threshold.xlsx
+++ b/outputs/threshold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanxinli/Desktop/project/BlindKameris-new/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6040964-10CB-2A4E-88E1-5C2DB306A259}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3CF076-BD2D-0542-9DB7-2CCFE6366C1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="7180" windowWidth="28040" windowHeight="15880" xr2:uid="{19BAD133-A47C-3C43-939A-0C9920B0410D}"/>
+    <workbookView xWindow="760" yWindow="480" windowWidth="28040" windowHeight="15880" xr2:uid="{19BAD133-A47C-3C43-939A-0C9920B0410D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="A8:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>